<commit_message>
Strings for Station IDs in templates allowed
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_multi.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_multi.xlsx
@@ -673,24 +673,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -712,6 +694,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -732,6 +721,17 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1109,12 +1109,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
-      <formula1>1</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
       <formula1>ToB</formula1>
     </dataValidation>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1158,43 +1156,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="48" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="43" t="s">
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="44"/>
-      <c r="O1" s="41" t="s">
+      <c r="N1" s="39"/>
+      <c r="O1" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="40" t="s">
         <v>83</v>
       </c>
       <c r="R1" s="51" t="s">
@@ -1209,24 +1207,24 @@
       <c r="U1" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="W1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
     </row>
     <row r="2" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
       <c r="E2" s="33" t="s">
         <v>82</v>
       </c>
@@ -1257,24 +1255,36 @@
       <c r="N2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="35"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="41"/>
       <c r="R2" s="52"/>
       <c r="S2" s="52"/>
       <c r="T2" s="52"/>
       <c r="U2" s="52"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1286,18 +1296,6 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576 M3:M1048576">

</xml_diff>